<commit_message>
support subjects when uploading examinee info
</commit_message>
<xml_diff>
--- a/src/assets/templates/考生列表.xlsx
+++ b/src/assets/templates/考生列表.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jet/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>姓名</t>
   </si>
@@ -48,16 +43,51 @@
   </si>
   <si>
     <t>王五</t>
+  </si>
+  <si>
+    <t>科目</t>
+  </si>
+  <si>
+    <t>语文,数学,英语</t>
+  </si>
+  <si>
+    <t>语文,数学,英语,物理,化学</t>
+  </si>
+  <si>
+    <t>语文,数学(文),英语,政治,历史</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,13 +110,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -142,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -177,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -354,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -362,15 +397,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,8 +422,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -397,8 +439,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -411,8 +456,11 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -424,9 +472,18 @@
       </c>
       <c r="D4" t="s">
         <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enhance the examinee batch template
</commit_message>
<xml_diff>
--- a/src/assets/templates/考生列表.xlsx
+++ b/src/assets/templates/考生列表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>姓名</t>
   </si>
@@ -54,7 +54,16 @@
     <t>语文,数学,英语,物理,化学</t>
   </si>
   <si>
-    <t>语文,数学(文),英语,政治,历史</t>
+    <t>科目列表1</t>
+  </si>
+  <si>
+    <t>科目列表2</t>
+  </si>
+  <si>
+    <t>科目列表3</t>
+  </si>
+  <si>
+    <t>语文,数学,英语,政治,历史</t>
   </si>
 </sst>
 </file>
@@ -110,8 +119,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -119,9 +136,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,7 +414,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -410,71 +435,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>186114</v>
-      </c>
-      <c r="C2">
-        <v>186114</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>186115</v>
-      </c>
-      <c r="C3">
-        <v>186115</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>186114</v>
+      </c>
+      <c r="C5">
+        <v>186114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>186115</v>
+      </c>
+      <c r="C6">
+        <v>186115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B7">
         <v>186116</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>186116</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
roll back the changes of batch uploading examinees
</commit_message>
<xml_diff>
--- a/src/assets/templates/考生列表.xlsx
+++ b/src/assets/templates/考生列表.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>姓名</t>
   </si>
@@ -54,16 +54,7 @@
     <t>语文,数学,英语,物理,化学</t>
   </si>
   <si>
-    <t>科目列表1</t>
-  </si>
-  <si>
-    <t>科目列表2</t>
-  </si>
-  <si>
-    <t>科目列表3</t>
-  </si>
-  <si>
-    <t>语文,数学,英语,政治,历史</t>
+    <t>语文,数学(文),英语,政治,历史</t>
   </si>
 </sst>
 </file>
@@ -119,16 +110,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -136,17 +119,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -422,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -435,95 +410,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>186114</v>
+      </c>
+      <c r="C2">
+        <v>186114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>186115</v>
+      </c>
+      <c r="C3">
+        <v>186115</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>186116</v>
+      </c>
+      <c r="C4">
+        <v>186116</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>186114</v>
-      </c>
-      <c r="C5">
-        <v>186114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>186115</v>
-      </c>
-      <c r="C6">
-        <v>186115</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>186116</v>
-      </c>
-      <c r="C7">
-        <v>186116</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>